<commit_message>
Merged PR 9770: When there is a null in the rows to merge then it is always returning false.
When there is a null in the rows to merge then it is always returning false.

Related work items: #55500
</commit_message>
<xml_diff>
--- a/CalculateFunding.Services.Datasets.UnitTests/TestItems/PE_and_Sports_Grant_Data_result.xlsx
+++ b/CalculateFunding.Services.Datasets.UnitTests/TestItems/PE_and_Sports_Grant_Data_result.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rohit\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\CFS\CalculateFunding-Backend\CalculateFunding.Services.Datasets.UnitTests\TestItems\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{250E8BB5-BC96-4B54-9F2E-069F0394C0B2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{57B7396A-F3FF-4516-995C-06361D01A5F5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="13152" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="PE and Sport Grant" sheetId="1" r:id="rId1"/>
@@ -1079,21 +1079,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:U93"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H12" sqref="H12"/>
+    <sheetView tabSelected="1" topLeftCell="S1" workbookViewId="0">
+      <selection activeCell="U3" sqref="U3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="3" width="9.1796875" customWidth="1"/>
-    <col min="4" max="4" width="9.453125" customWidth="1"/>
-    <col min="5" max="5" width="14.08984375" customWidth="1"/>
-    <col min="6" max="6" width="13.1796875" customWidth="1"/>
-    <col min="7" max="7" width="11.81640625" customWidth="1"/>
-    <col min="8" max="8" width="18.453125" customWidth="1"/>
-    <col min="9" max="14" width="58.453125" customWidth="1"/>
-    <col min="15" max="20" width="42.54296875" customWidth="1"/>
-    <col min="21" max="21" width="71.6328125" customWidth="1"/>
+    <col min="1" max="3" width="9.15625" customWidth="1"/>
+    <col min="4" max="4" width="9.47265625" customWidth="1"/>
+    <col min="5" max="5" width="14.1015625" customWidth="1"/>
+    <col min="6" max="6" width="13.15625" customWidth="1"/>
+    <col min="7" max="7" width="11.7890625" customWidth="1"/>
+    <col min="8" max="8" width="18.47265625" customWidth="1"/>
+    <col min="9" max="14" width="58.47265625" customWidth="1"/>
+    <col min="15" max="20" width="42.5234375" customWidth="1"/>
+    <col min="21" max="21" width="71.62890625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:21">
@@ -1220,9 +1220,6 @@
         <v>0</v>
       </c>
       <c r="T2">
-        <v>0</v>
-      </c>
-      <c r="U2">
         <v>0</v>
       </c>
     </row>
@@ -7154,7 +7151,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" t="s">
@@ -7202,12 +7199,9 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -7420,15 +7414,27 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{893FC4BE-952F-4B77-A17C-02E1E16AD86B}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BA5BD8A6-8524-4FB3-BADC-0E49138F02CE}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="7e3e27cc-3a1c-477d-aac6-02b314d79f5e"/>
+    <ds:schemaRef ds:uri="ab119141-cd66-4087-86bb-8e659032e627"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -7453,18 +7459,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BA5BD8A6-8524-4FB3-BADC-0E49138F02CE}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{893FC4BE-952F-4B77-A17C-02E1E16AD86B}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="7e3e27cc-3a1c-477d-aac6-02b314d79f5e"/>
-    <ds:schemaRef ds:uri="ab119141-cd66-4087-86bb-8e659032e627"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Merged PR 11706: Ensure changes on set as ignore merge dataset fieilds ignored
Ensure changes on set as ignore merge dataset fieilds ignored

Related work items: #64577
</commit_message>
<xml_diff>
--- a/CalculateFunding.Services.Datasets.UnitTests/TestItems/PE_and_Sports_Grant_Data_result.xlsx
+++ b/CalculateFunding.Services.Datasets.UnitTests/TestItems/PE_and_Sports_Grant_Data_result.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23929"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\CFS\CalculateFunding-Backend\CalculateFunding.Services.Datasets.UnitTests\TestItems\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\src\sinem\CalculateFunding-Backend\CalculateFunding.Services.Datasets.UnitTests\TestItems\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{57B7396A-F3FF-4516-995C-06361D01A5F5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{576B9ADC-27E2-4D3D-A813-F1B6F50A1BE3}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="13152" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="9600" yWindow="5380" windowWidth="28800" windowHeight="15290" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="PE and Sport Grant" sheetId="1" r:id="rId1"/>
@@ -1080,20 +1080,20 @@
   <dimension ref="A1:U93"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="S1" workbookViewId="0">
-      <selection activeCell="U3" sqref="U3"/>
+      <selection activeCell="T8" sqref="T8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="3" width="9.15625" customWidth="1"/>
-    <col min="4" max="4" width="9.47265625" customWidth="1"/>
-    <col min="5" max="5" width="14.1015625" customWidth="1"/>
-    <col min="6" max="6" width="13.15625" customWidth="1"/>
-    <col min="7" max="7" width="11.7890625" customWidth="1"/>
-    <col min="8" max="8" width="18.47265625" customWidth="1"/>
-    <col min="9" max="14" width="58.47265625" customWidth="1"/>
-    <col min="15" max="20" width="42.5234375" customWidth="1"/>
-    <col min="21" max="21" width="71.62890625" customWidth="1"/>
+    <col min="1" max="3" width="9.1796875" customWidth="1"/>
+    <col min="4" max="4" width="9.453125" customWidth="1"/>
+    <col min="5" max="5" width="14.08984375" customWidth="1"/>
+    <col min="6" max="6" width="13.1796875" customWidth="1"/>
+    <col min="7" max="7" width="11.81640625" customWidth="1"/>
+    <col min="8" max="8" width="18.453125" customWidth="1"/>
+    <col min="9" max="14" width="58.453125" customWidth="1"/>
+    <col min="15" max="20" width="42.54296875" customWidth="1"/>
+    <col min="21" max="21" width="71.6328125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:21">
@@ -7151,7 +7151,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" t="s">
@@ -7199,9 +7199,12 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -7414,27 +7417,15 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BA5BD8A6-8524-4FB3-BADC-0E49138F02CE}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{893FC4BE-952F-4B77-A17C-02E1E16AD86B}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="7e3e27cc-3a1c-477d-aac6-02b314d79f5e"/>
-    <ds:schemaRef ds:uri="ab119141-cd66-4087-86bb-8e659032e627"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -7459,9 +7450,18 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{893FC4BE-952F-4B77-A17C-02E1E16AD86B}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BA5BD8A6-8524-4FB3-BADC-0E49138F02CE}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="7e3e27cc-3a1c-477d-aac6-02b314d79f5e"/>
+    <ds:schemaRef ds:uri="ab119141-cd66-4087-86bb-8e659032e627"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>